<commit_message>
convert scripts to funcs
</commit_message>
<xml_diff>
--- a/Examples/Børne Klub 100/Børne Klub 100.xlsx
+++ b/Examples/Børne Klub 100/Børne Klub 100.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72ad7a60f2949dc8/Dokumenter/DTU/Vektor/klub-100-maker/Examples/Børne Klub 100/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Dokumenter\DTU\Vektor\klub-100-maker\Examples\Børne Klub 100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B74159E1-9D3A-4209-AA41-EACA3A224F82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B74159E1-9D3A-4209-AA41-EACA3A224F82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{5EAFEE2E-C7AB-4B3B-A49A-542EF3F40A9F}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="11586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Shoutout titel</t>
   </si>
   <si>
-    <t>Sang - Kunster</t>
-  </si>
-  <si>
     <t>Shoutouts</t>
   </si>
   <si>
@@ -1000,6 +997,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=bnw3Dywvs2s&amp;list=PLVZFxulTtgNO64S-jrop7Sqw2Lq2Qan59&amp;index=194</t>
+  </si>
+  <si>
+    <t>Sang - Kunstner</t>
   </si>
 </sst>
 </file>
@@ -1314,41 +1314,41 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>322</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C2" s="1">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -1356,10 +1356,10 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1">
         <v>25</v>
@@ -1367,10 +1367,10 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>33</v>
       </c>
       <c r="C5" s="1">
         <v>50</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -1389,10 +1389,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>20</v>
@@ -1400,24 +1400,24 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="C9" s="1">
         <v>10</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -1436,24 +1436,24 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1">
         <v>55</v>
@@ -1461,10 +1461,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="C13" s="1">
         <v>43</v>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C14" s="1">
         <v>40</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>73</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1494,10 +1494,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1">
         <v>15</v>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>80</v>
       </c>
       <c r="C18" s="1">
         <v>7</v>
@@ -1516,24 +1516,24 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1541,10 +1541,10 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
@@ -1552,10 +1552,10 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="1">
         <v>0</v>
@@ -1563,10 +1563,10 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="C24" s="1">
         <v>10</v>
@@ -1574,10 +1574,10 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>116</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="C25" s="1">
         <v>0</v>
@@ -1585,10 +1585,10 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>119</v>
       </c>
       <c r="C26" s="1">
         <v>0</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="C27" s="1">
         <v>0</v>
@@ -1607,10 +1607,10 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="C28" s="1">
         <v>0</v>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>128</v>
       </c>
       <c r="C29" s="1">
         <v>0</v>
@@ -1629,10 +1629,10 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="C30" s="1">
         <v>0</v>
@@ -1640,10 +1640,10 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="C31" s="1">
         <v>0</v>
@@ -1651,10 +1651,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>135</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -1662,10 +1662,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>139</v>
       </c>
       <c r="C33" s="1">
         <v>0</v>
@@ -1673,10 +1673,10 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="C34" s="1">
         <v>0</v>
@@ -1684,10 +1684,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="C35" s="1">
         <v>0</v>
@@ -1695,10 +1695,10 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="C36" s="1">
         <v>76</v>
@@ -1706,10 +1706,10 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="C37" s="1">
         <v>0</v>
@@ -1717,10 +1717,10 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>162</v>
       </c>
       <c r="C38" s="1">
         <v>6</v>
@@ -1728,10 +1728,10 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C39" s="1">
         <v>0</v>
@@ -1739,10 +1739,10 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="C40" s="1">
         <v>0</v>
@@ -1750,38 +1750,38 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>173</v>
-      </c>
       <c r="C42" s="1">
         <v>0</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>176</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>177</v>
       </c>
       <c r="C43" s="1">
         <v>0</v>
@@ -1789,10 +1789,10 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>179</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
@@ -1800,24 +1800,24 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C45" s="1">
-        <v>0</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B46" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="C46" s="1">
         <v>0</v>
@@ -1825,10 +1825,10 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>186</v>
       </c>
       <c r="C47" s="1">
         <v>6</v>
@@ -1836,10 +1836,10 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>188</v>
       </c>
       <c r="C48" s="1">
         <v>3</v>
@@ -1847,10 +1847,10 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>190</v>
       </c>
       <c r="C49" s="1">
         <v>13</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="C50" s="1">
         <v>20</v>
@@ -1869,10 +1869,10 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B51" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="C51" s="1">
         <v>3</v>
@@ -1880,10 +1880,10 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>195</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>196</v>
       </c>
       <c r="C52" s="1">
         <v>0</v>
@@ -1891,10 +1891,10 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>198</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
@@ -1902,10 +1902,10 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="C54" s="1">
         <v>0</v>
@@ -1913,24 +1913,24 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C56" s="1">
-        <v>0</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>205</v>
       </c>
       <c r="C57" s="1">
         <v>0</v>
@@ -1938,10 +1938,10 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B58" s="5" t="s">
         <v>206</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>207</v>
       </c>
       <c r="C58" s="1">
         <v>50</v>
@@ -1949,10 +1949,10 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>209</v>
       </c>
       <c r="C59" s="1">
         <v>46</v>
@@ -1960,10 +1960,10 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="C60" s="1">
         <v>0</v>
@@ -1971,10 +1971,10 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B61" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="C61" s="1">
         <v>38</v>
@@ -1982,10 +1982,10 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>215</v>
       </c>
       <c r="C62" s="1">
         <v>3</v>
@@ -1993,10 +1993,10 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>217</v>
       </c>
       <c r="C63" s="1">
         <v>5</v>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>219</v>
       </c>
       <c r="C64" s="1">
         <v>11</v>
@@ -2015,10 +2015,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>220</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>221</v>
       </c>
       <c r="C65" s="1">
         <v>0</v>
@@ -2026,10 +2026,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>223</v>
       </c>
       <c r="C66" s="1">
         <v>0</v>
@@ -2037,10 +2037,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B67" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="B67" s="5" t="s">
-        <v>225</v>
       </c>
       <c r="C67" s="1">
         <v>15</v>
@@ -2048,10 +2048,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>226</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>227</v>
       </c>
       <c r="C68" s="1">
         <v>0</v>
@@ -2059,10 +2059,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B69" s="6" t="s">
         <v>228</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>229</v>
       </c>
       <c r="C69" s="1">
         <v>6</v>
@@ -2070,10 +2070,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B70" s="6" t="s">
         <v>230</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>231</v>
       </c>
       <c r="C70" s="1">
         <v>0</v>
@@ -2081,10 +2081,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>232</v>
-      </c>
-      <c r="B71" s="5" t="s">
-        <v>233</v>
       </c>
       <c r="C71" s="1">
         <v>30</v>
@@ -2092,10 +2092,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>234</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>235</v>
       </c>
       <c r="C72" s="1">
         <v>50</v>
@@ -2103,10 +2103,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B73" s="6" t="s">
         <v>236</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>237</v>
       </c>
       <c r="C73" s="1">
         <v>0</v>
@@ -2114,10 +2114,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>239</v>
       </c>
       <c r="C74" s="1">
         <v>5</v>
@@ -2125,10 +2125,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B75" s="6" t="s">
         <v>240</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>241</v>
       </c>
       <c r="C75" s="1">
         <v>0</v>
@@ -2136,10 +2136,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B76" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>243</v>
       </c>
       <c r="C76" s="1">
         <v>75</v>
@@ -2147,10 +2147,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>245</v>
       </c>
       <c r="C77" s="1">
         <v>3</v>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B78" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>247</v>
       </c>
       <c r="C78" s="1">
         <v>10</v>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B79" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="B79" s="5" t="s">
-        <v>249</v>
       </c>
       <c r="C79" s="1">
         <v>32</v>
@@ -2180,10 +2180,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>250</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>251</v>
       </c>
       <c r="C80" s="1">
         <v>0</v>
@@ -2191,10 +2191,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>253</v>
       </c>
       <c r="C81" s="1">
         <v>6</v>
@@ -2202,10 +2202,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B82" s="6" t="s">
         <v>254</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="C82" s="1">
         <v>0</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>256</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>257</v>
       </c>
       <c r="C83" s="1">
         <v>0</v>
@@ -2224,10 +2224,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B84" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="B84" s="5" t="s">
-        <v>259</v>
       </c>
       <c r="C84" s="1">
         <v>0</v>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>260</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>261</v>
       </c>
       <c r="C85" s="1">
         <v>0</v>
@@ -2246,10 +2246,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>263</v>
       </c>
       <c r="C86" s="1">
         <v>0</v>
@@ -2257,18 +2257,18 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B87" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B88" s="5" t="s">
         <v>266</v>
-      </c>
-      <c r="B88" s="5" t="s">
-        <v>267</v>
       </c>
       <c r="C88" s="1">
         <v>0</v>
@@ -2276,10 +2276,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="C90" s="1">
         <v>18</v>
@@ -2287,10 +2287,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B91" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="B91" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="C91" s="1">
         <v>0</v>
@@ -2298,10 +2298,10 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B92" s="5" t="s">
         <v>272</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>273</v>
       </c>
       <c r="C92" s="1">
         <v>10</v>
@@ -2309,10 +2309,10 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B93" s="5" t="s">
         <v>274</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>275</v>
       </c>
       <c r="C93" s="1">
         <v>0</v>
@@ -2320,10 +2320,10 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B96" s="6" t="s">
         <v>276</v>
-      </c>
-      <c r="B96" s="6" t="s">
-        <v>277</v>
       </c>
       <c r="C96" s="1">
         <v>19</v>
@@ -2331,10 +2331,10 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B98" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="C98" s="1">
         <v>0</v>
@@ -2342,10 +2342,10 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B99" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="C99" s="1">
         <v>70</v>
@@ -2353,10 +2353,10 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B100" s="6" t="s">
         <v>282</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>283</v>
       </c>
       <c r="C100" s="1">
         <v>0</v>
@@ -2364,32 +2364,32 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B101" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="C101" s="1">
         <v>18</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B104" s="6" t="s">
         <v>288</v>
-      </c>
-      <c r="B104" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="C104" s="1">
         <v>0</v>
@@ -2397,24 +2397,24 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B105" s="5" t="s">
         <v>290</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>291</v>
       </c>
       <c r="C105" s="1">
         <v>80</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B106" s="6" t="s">
         <v>293</v>
-      </c>
-      <c r="B106" s="6" t="s">
-        <v>294</v>
       </c>
       <c r="C106" s="1">
         <v>0</v>
@@ -2422,10 +2422,10 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="C107" s="1">
         <v>15</v>
@@ -2433,10 +2433,10 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B108" s="6" t="s">
         <v>297</v>
-      </c>
-      <c r="B108" s="6" t="s">
-        <v>298</v>
       </c>
       <c r="C108" s="1">
         <v>0</v>
@@ -2444,10 +2444,10 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>299</v>
-      </c>
-      <c r="B109" s="5" t="s">
-        <v>300</v>
       </c>
       <c r="C109" s="1">
         <v>0</v>
@@ -2455,10 +2455,10 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="B110" s="5" t="s">
-        <v>302</v>
       </c>
       <c r="C110" s="1">
         <v>6</v>
@@ -2466,10 +2466,10 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B111" s="6" t="s">
         <v>303</v>
-      </c>
-      <c r="B111" s="6" t="s">
-        <v>304</v>
       </c>
       <c r="C111" s="1">
         <v>0</v>
@@ -2477,10 +2477,10 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B112" s="6" t="s">
         <v>305</v>
-      </c>
-      <c r="B112" s="6" t="s">
-        <v>306</v>
       </c>
       <c r="C112" s="1">
         <v>0</v>
@@ -2488,10 +2488,10 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B113" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="C113" s="1">
         <v>198</v>
@@ -2499,10 +2499,10 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B114" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="C114" s="1">
         <v>17</v>
@@ -2510,10 +2510,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B115" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="B115" s="6" t="s">
-        <v>312</v>
       </c>
       <c r="C115" s="1">
         <v>5</v>
@@ -2521,10 +2521,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B116" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>314</v>
       </c>
       <c r="C116" s="1">
         <v>0</v>
@@ -2532,10 +2532,10 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B117" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="B117" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="C117" s="1">
         <v>0</v>
@@ -2543,10 +2543,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B118" s="5" t="s">
         <v>317</v>
-      </c>
-      <c r="B118" s="5" t="s">
-        <v>318</v>
       </c>
       <c r="C118" s="1">
         <v>0</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="B119" s="5" t="s">
         <v>319</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>320</v>
       </c>
       <c r="C119" s="1">
         <v>0</v>
@@ -2565,10 +2565,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="B120" s="5" t="s">
         <v>321</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>322</v>
       </c>
       <c r="C120" s="1">
         <v>6</v>
@@ -2713,44 +2713,44 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="4">
         <f>9*60+21</f>
@@ -2761,18 +2761,18 @@
         <v>573</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="E5" s="1">
         <v>31</v>
@@ -2781,13 +2781,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E6" s="1">
         <v>39</v>
@@ -2798,16 +2798,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D7" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E7" s="1">
         <v>20</v>
@@ -2818,13 +2818,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="E8" s="1">
         <v>266</v>
@@ -2835,13 +2835,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
         <v>57</v>
@@ -2852,13 +2852,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="E10" s="1">
         <v>183</v>
@@ -2869,13 +2869,13 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="E11" s="1">
         <v>378</v>
@@ -2886,13 +2886,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E12" s="1">
         <v>185</v>
@@ -2903,13 +2903,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="E13" s="1">
         <v>49</v>
@@ -2918,18 +2918,18 @@
         <v>69</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>95</v>
       </c>
       <c r="E14" s="1">
         <v>686</v>
@@ -2938,18 +2938,18 @@
         <v>707</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="E15" s="1">
         <f>6*60+42</f>
@@ -2962,13 +2962,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="E16" s="1">
         <f>13*60+55</f>
@@ -2981,13 +2981,13 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="E17" s="1">
         <f>5*60+25</f>
@@ -3000,13 +3000,13 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>125</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="E18" s="4">
         <f>3*60+44</f>
@@ -3018,13 +3018,13 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E19" s="4">
         <f>9*60+55</f>
@@ -3036,13 +3036,13 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="E20" s="4">
         <f>13*60+24</f>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="D21" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>142</v>
       </c>
       <c r="E21" s="1">
         <v>149</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="D22" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="E22" s="1">
         <v>28</v>
@@ -3089,13 +3089,13 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="D23" s="5" t="s">
         <v>151</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>152</v>
       </c>
       <c r="E23" s="1">
         <v>61</v>
@@ -3106,13 +3106,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>156</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -3120,13 +3120,13 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>160</v>
       </c>
       <c r="E25" s="1">
         <v>70</v>
@@ -3135,18 +3135,18 @@
         <v>87</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="E26" s="4">
         <f>7*60+7</f>
@@ -3159,13 +3159,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E27" s="1">
         <v>175</v>
@@ -3221,12 +3221,12 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
         <f>COUNTIFS(Sange!A2:A1000, "*", Sange!B2:B1000, "*", Sange!C2:C1000, "&gt;=0")</f>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" ref="B3:C3" si="0">B4-B2</f>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4">
         <f>COUNTIF(Sange!A3:A1000, "*")</f>
@@ -3265,7 +3265,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="4">
         <f>COUNTIFS(Ideer!A2:A1000, "Sang", Ideer!B2:B1000, "*")</f>
@@ -3298,66 +3298,66 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="E3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="4"/>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5">

</xml_diff>